<commit_message>
updating test data for upcoming tests
</commit_message>
<xml_diff>
--- a/testdata/test1.xlsx
+++ b/testdata/test1.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashib\PycharmProjects\SelPyHybridFramework\excelfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashib\OneDrive\Desktop\local_repo\CloudEcomAutomation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C7B3F8-9253-4FDD-B058-C508E6260187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1A184C-3EEE-456F-A063-6672DC81E266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="4068" windowWidth="17280" windowHeight="9828" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login_test" sheetId="2" r:id="rId1"/>
     <sheet name="register_test" sheetId="3" r:id="rId2"/>
+    <sheet name="payment_address" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -48,6 +49,45 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>post_code</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testing address1</t>
+  </si>
+  <si>
+    <t>test city</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
   </si>
 </sst>
 </file>
@@ -483,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CABA58-8F72-4E3C-B78E-A51159C4E841}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,4 +549,68 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E42B529-F04A-484B-9625-63BE3D3A6BA6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5">
+        <v>54645</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>